<commit_message>
New Zenodo link to new corrected IMAGE files
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-cdr-cement-mineralization.xlsx
+++ b/premise/data/additional_inventories/lci-cdr-cement-mineralization.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EAECFDB-A786-D34E-AD35-9643A8B1AAC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F921F65B-8B69-634E-A81A-26020F9F03B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -785,8 +785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="165" zoomScaleNormal="289" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="165" zoomScaleNormal="289" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1108,8 +1108,8 @@
         <v>carbon dioxide evaporation, for cement mineralization</v>
       </c>
       <c r="B21" s="10">
-        <f>B88+B20</f>
-        <v>1.1052631578947367</v>
+        <f>1+B20</f>
+        <v>1.0526315789473684</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>3</v>

</xml_diff>